<commit_message>
fix(condo): DOMA-11339 fixed tests and example files
</commit_message>
<xml_diff>
--- a/apps/condo/domains/meter/tasks/mock-files/meter-import-example-excel-date-type-en.xlsx
+++ b/apps/condo/domains/meter/tasks/mock-files/meter-import-example-excel-date-type-en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>Address</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Automatic</t>
+  </si>
+  <si>
+    <t>Decommissioning date</t>
   </si>
   <si>
     <t>Moscow city, ulitsa Tverskaya, dom 1</t>
@@ -157,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -226,80 +229,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -355,33 +291,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="64" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1440,7 +1349,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1460,8 +1369,8 @@
     <col min="15" max="15" width="12.8516" style="1" customWidth="1"/>
     <col min="16" max="16" width="22.1719" style="1" customWidth="1"/>
     <col min="17" max="17" width="18.1719" style="1" customWidth="1"/>
-    <col min="18" max="20" width="23.5" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="18" max="21" width="23.5" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.75" customHeight="1">
@@ -1525,25 +1434,28 @@
       <c r="T1" t="s" s="7">
         <v>19</v>
       </c>
+      <c r="U1" t="s" s="7">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" ht="13.75" customHeight="1">
       <c r="A2" t="s" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s" s="9">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s" s="9">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s" s="9">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s" s="9">
         <v>22</v>
-      </c>
-      <c r="D2" t="s" s="9">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s" s="9">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s" s="9">
-        <v>21</v>
       </c>
       <c r="G2" s="10">
         <v>1</v>
@@ -1576,185 +1488,10 @@
         <v>44550.466099537036</v>
       </c>
       <c r="S2" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T2" s="7"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="21"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="24"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="24"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="24"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="24"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="24"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="24"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="27"/>
+      <c r="U2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
fix(condo): DOMA-11339 added archiveDate field in meters import (#5962)
* fix(condo): DOMA-11339 added archiveDate field in meters import

* fix(condo): DOMA-11339 fixed tests and example files
</commit_message>
<xml_diff>
--- a/apps/condo/domains/meter/tasks/mock-files/meter-import-example-excel-date-type-en.xlsx
+++ b/apps/condo/domains/meter/tasks/mock-files/meter-import-example-excel-date-type-en.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>Address</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t>Automatic</t>
+  </si>
+  <si>
+    <t>Decommissioning date</t>
   </si>
   <si>
     <t>Moscow city, ulitsa Tverskaya, dom 1</t>
@@ -157,7 +160,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -226,80 +229,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="11"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="11"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -355,33 +291,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="64" fontId="0" fillId="4" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1440,7 +1349,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1460,8 +1369,8 @@
     <col min="15" max="15" width="12.8516" style="1" customWidth="1"/>
     <col min="16" max="16" width="22.1719" style="1" customWidth="1"/>
     <col min="17" max="17" width="18.1719" style="1" customWidth="1"/>
-    <col min="18" max="20" width="23.5" style="1" customWidth="1"/>
-    <col min="21" max="16384" width="14.5" style="1" customWidth="1"/>
+    <col min="18" max="21" width="23.5" style="1" customWidth="1"/>
+    <col min="22" max="16384" width="14.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.75" customHeight="1">
@@ -1525,25 +1434,28 @@
       <c r="T1" t="s" s="7">
         <v>19</v>
       </c>
+      <c r="U1" t="s" s="7">
+        <v>20</v>
+      </c>
     </row>
     <row r="2" ht="13.75" customHeight="1">
       <c r="A2" t="s" s="8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s" s="9">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s" s="9">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s" s="9">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s" s="9">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s" s="9">
         <v>22</v>
-      </c>
-      <c r="D2" t="s" s="9">
-        <v>23</v>
-      </c>
-      <c r="E2" t="s" s="9">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s" s="9">
-        <v>21</v>
       </c>
       <c r="G2" s="10">
         <v>1</v>
@@ -1576,185 +1488,10 @@
         <v>44550.466099537036</v>
       </c>
       <c r="S2" t="s" s="7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="T2" s="7"/>
-    </row>
-    <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" s="19"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="20"/>
-      <c r="S3" s="20"/>
-      <c r="T3" s="21"/>
-    </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" s="22"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="23"/>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
-      <c r="R4" s="23"/>
-      <c r="S4" s="23"/>
-      <c r="T4" s="24"/>
-    </row>
-    <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" s="22"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="24"/>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="24"/>
-    </row>
-    <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="24"/>
-    </row>
-    <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="24"/>
-    </row>
-    <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
-      <c r="S9" s="23"/>
-      <c r="T9" s="24"/>
-    </row>
-    <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="27"/>
+      <c r="U2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>